<commit_message>
first commit  in pingan
</commit_message>
<xml_diff>
--- a/resource/tsl_tableinfo.xlsx
+++ b/resource/tsl_tableinfo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{47F1D327-7ECB-455B-B612-76FAF9719624}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9403DE8-2636-4FE3-93F5-F29E01CD046F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FactorID" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="481">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1568,6 +1568,114 @@
   </si>
   <si>
     <t>801204.SW</t>
+  </si>
+  <si>
+    <t>截止日</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shares_hold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>占总股本比例(%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ratio_hold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买入金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卖出金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买入及卖出金额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>排名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amt_buy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amt_sell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>amt_trade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stock_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>股票名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卖出成交额(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买入成交额(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买入及卖出成交额(元)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买入成交数目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卖出成交数目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买入及卖出成交数目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vol_buy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vol_sell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vol_trade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1928,22 +2036,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F79"/>
+  <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.25" customWidth="1"/>
-    <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1963,7 +2071,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1977,7 +2085,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1991,7 +2099,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2005,7 +2113,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -2019,7 +2127,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -2033,7 +2141,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -2047,7 +2155,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2061,7 +2169,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2075,7 +2183,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2089,7 +2197,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -2103,7 +2211,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -2117,7 +2225,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2131,7 +2239,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2145,7 +2253,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2159,7 +2267,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2173,7 +2281,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2187,7 +2295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2201,7 +2309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2215,7 +2323,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2229,7 +2337,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2243,7 +2351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2257,7 +2365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2271,7 +2379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2285,7 +2393,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2299,7 +2407,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2313,7 +2421,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2327,7 +2435,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2341,7 +2449,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -2358,7 +2466,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -2375,7 +2483,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2392,7 +2500,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2409,7 +2517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -2426,7 +2534,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -2443,7 +2551,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
@@ -2460,7 +2568,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -2477,7 +2585,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>126</v>
       </c>
@@ -2494,7 +2602,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>127</v>
       </c>
@@ -2511,7 +2619,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -2528,7 +2636,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -2545,7 +2653,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -2562,7 +2670,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -2579,7 +2687,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>77</v>
       </c>
@@ -2596,7 +2704,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>80</v>
       </c>
@@ -2610,7 +2718,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>81</v>
       </c>
@@ -2624,7 +2732,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -2638,7 +2746,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>83</v>
       </c>
@@ -2652,7 +2760,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>84</v>
       </c>
@@ -2666,7 +2774,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>89</v>
       </c>
@@ -2680,7 +2788,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2694,7 +2802,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -2708,7 +2816,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>92</v>
       </c>
@@ -2722,7 +2830,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>93</v>
       </c>
@@ -2736,7 +2844,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>94</v>
       </c>
@@ -2750,7 +2858,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>95</v>
       </c>
@@ -2764,7 +2872,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>96</v>
       </c>
@@ -2778,7 +2886,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>97</v>
       </c>
@@ -2792,7 +2900,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>98</v>
       </c>
@@ -2806,7 +2914,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>109</v>
       </c>
@@ -2826,7 +2934,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>113</v>
       </c>
@@ -2846,7 +2954,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>117</v>
       </c>
@@ -2866,7 +2974,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>120</v>
       </c>
@@ -2886,7 +2994,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>124</v>
       </c>
@@ -2906,7 +3014,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>47</v>
       </c>
@@ -2923,7 +3031,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>48</v>
       </c>
@@ -2940,7 +3048,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>49</v>
       </c>
@@ -2957,7 +3065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>46</v>
       </c>
@@ -2974,7 +3082,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>50</v>
       </c>
@@ -2991,7 +3099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>51</v>
       </c>
@@ -3008,7 +3116,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>58</v>
       </c>
@@ -3025,7 +3133,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -3042,7 +3150,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>126</v>
       </c>
@@ -3062,7 +3170,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>127</v>
       </c>
@@ -3082,7 +3190,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>144</v>
       </c>
@@ -3102,7 +3210,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>149</v>
       </c>
@@ -3122,7 +3230,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>151</v>
       </c>
@@ -3142,7 +3250,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>154</v>
       </c>
@@ -3162,7 +3270,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>157</v>
       </c>
@@ -3182,7 +3290,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>161</v>
       </c>
@@ -3200,6 +3308,244 @@
       </c>
       <c r="F79" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>454</v>
+      </c>
+      <c r="B80">
+        <v>132001</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D80">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>456</v>
+      </c>
+      <c r="B81">
+        <v>132002</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D81">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>458</v>
+      </c>
+      <c r="B82">
+        <v>132003</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D82">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>454</v>
+      </c>
+      <c r="B83">
+        <v>131001</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D83">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>460</v>
+      </c>
+      <c r="B84">
+        <v>131002</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D84">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>471</v>
+      </c>
+      <c r="B85">
+        <v>131003</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D85">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>461</v>
+      </c>
+      <c r="B86">
+        <v>131004</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D86">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>462</v>
+      </c>
+      <c r="B87">
+        <v>131005</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D87">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>463</v>
+      </c>
+      <c r="B88">
+        <v>131006</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D88">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>464</v>
+      </c>
+      <c r="B89">
+        <v>131007</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D89">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>454</v>
+      </c>
+      <c r="B90">
+        <v>130001</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D90">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>472</v>
+      </c>
+      <c r="B91">
+        <v>130004</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D91">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>473</v>
+      </c>
+      <c r="B92">
+        <v>130003</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D92">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>474</v>
+      </c>
+      <c r="B93">
+        <v>130002</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D93">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>475</v>
+      </c>
+      <c r="B94">
+        <v>130009</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D94">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>476</v>
+      </c>
+      <c r="B95">
+        <v>130010</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D95">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>477</v>
+      </c>
+      <c r="B96">
+        <v>130011</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D96">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -3217,13 +3563,13 @@
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3231,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3239,7 +3585,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3247,7 +3593,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3255,7 +3601,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -3263,7 +3609,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -3271,7 +3617,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -3279,7 +3625,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -3287,7 +3633,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -3295,7 +3641,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -3303,7 +3649,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -3311,7 +3657,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -3319,7 +3665,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>188</v>
       </c>
@@ -3327,7 +3673,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>189</v>
       </c>
@@ -3335,7 +3681,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>192</v>
       </c>
@@ -3343,7 +3689,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>237</v>
       </c>
@@ -3351,7 +3697,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>238</v>
       </c>
@@ -3359,7 +3705,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>240</v>
       </c>
@@ -3367,7 +3713,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>193</v>
       </c>
@@ -3375,7 +3721,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>241</v>
       </c>
@@ -3383,7 +3729,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>194</v>
       </c>
@@ -3391,7 +3737,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>195</v>
       </c>
@@ -3399,7 +3745,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>196</v>
       </c>
@@ -3407,7 +3753,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>197</v>
       </c>
@@ -3415,7 +3761,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>198</v>
       </c>
@@ -3423,7 +3769,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>199</v>
       </c>
@@ -3431,7 +3777,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>200</v>
       </c>
@@ -3439,7 +3785,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>242</v>
       </c>
@@ -3447,7 +3793,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>201</v>
       </c>
@@ -3455,7 +3801,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -3463,7 +3809,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>244</v>
       </c>
@@ -3471,7 +3817,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>203</v>
       </c>
@@ -3479,7 +3825,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>204</v>
       </c>
@@ -3487,7 +3833,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>205</v>
       </c>
@@ -3495,7 +3841,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>206</v>
       </c>
@@ -3503,7 +3849,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>245</v>
       </c>
@@ -3511,7 +3857,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>246</v>
       </c>
@@ -3519,7 +3865,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>247</v>
       </c>
@@ -3527,7 +3873,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>249</v>
       </c>
@@ -3535,7 +3881,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>207</v>
       </c>
@@ -3543,7 +3889,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>250</v>
       </c>
@@ -3551,7 +3897,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>208</v>
       </c>
@@ -3559,7 +3905,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>251</v>
       </c>
@@ -3567,7 +3913,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>252</v>
       </c>
@@ -3575,7 +3921,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>253</v>
       </c>
@@ -3583,7 +3929,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>254</v>
       </c>
@@ -3591,7 +3937,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>255</v>
       </c>
@@ -3599,7 +3945,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>256</v>
       </c>
@@ -3607,7 +3953,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>257</v>
       </c>
@@ -3615,7 +3961,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>258</v>
       </c>
@@ -3623,7 +3969,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>259</v>
       </c>
@@ -3631,7 +3977,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>260</v>
       </c>
@@ -3639,7 +3985,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>261</v>
       </c>
@@ -3647,7 +3993,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>262</v>
       </c>
@@ -3655,7 +4001,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>263</v>
       </c>
@@ -3663,7 +4009,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>264</v>
       </c>
@@ -3671,7 +4017,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>265</v>
       </c>
@@ -3679,7 +4025,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>266</v>
       </c>
@@ -3687,7 +4033,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>267</v>
       </c>
@@ -3695,7 +4041,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>268</v>
       </c>
@@ -3703,7 +4049,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>239</v>
       </c>
@@ -3711,7 +4057,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>269</v>
       </c>
@@ -3719,7 +4065,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>270</v>
       </c>
@@ -3727,7 +4073,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>271</v>
       </c>
@@ -3735,7 +4081,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>272</v>
       </c>
@@ -3743,7 +4089,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>273</v>
       </c>
@@ -3751,7 +4097,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>274</v>
       </c>
@@ -3759,7 +4105,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
@@ -3767,7 +4113,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>276</v>
       </c>
@@ -3775,7 +4121,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>277</v>
       </c>
@@ -3783,7 +4129,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>278</v>
       </c>
@@ -3791,7 +4137,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>279</v>
       </c>
@@ -3799,7 +4145,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>280</v>
       </c>
@@ -3807,7 +4153,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>281</v>
       </c>
@@ -3815,7 +4161,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>282</v>
       </c>
@@ -3823,7 +4169,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>283</v>
       </c>
@@ -3831,7 +4177,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>284</v>
       </c>
@@ -3839,7 +4185,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>285</v>
       </c>
@@ -3847,7 +4193,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>286</v>
       </c>
@@ -3855,7 +4201,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>287</v>
       </c>
@@ -3863,7 +4209,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>288</v>
       </c>
@@ -3871,7 +4217,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>289</v>
       </c>
@@ -3879,7 +4225,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>290</v>
       </c>
@@ -3887,7 +4233,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>291</v>
       </c>
@@ -3895,7 +4241,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>292</v>
       </c>
@@ -3903,7 +4249,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>293</v>
       </c>
@@ -3911,7 +4257,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>294</v>
       </c>
@@ -3919,7 +4265,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>295</v>
       </c>
@@ -3927,7 +4273,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>296</v>
       </c>
@@ -3935,7 +4281,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>297</v>
       </c>
@@ -3943,7 +4289,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>298</v>
       </c>
@@ -3951,7 +4297,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>299</v>
       </c>
@@ -3959,7 +4305,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>300</v>
       </c>
@@ -3967,7 +4313,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>301</v>
       </c>
@@ -3975,7 +4321,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>302</v>
       </c>
@@ -3983,7 +4329,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>303</v>
       </c>
@@ -3991,7 +4337,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>304</v>
       </c>
@@ -3999,7 +4345,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>305</v>
       </c>
@@ -4007,7 +4353,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>306</v>
       </c>
@@ -4015,7 +4361,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>307</v>
       </c>
@@ -4023,7 +4369,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>308</v>
       </c>
@@ -4031,7 +4377,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>309</v>
       </c>
@@ -4039,7 +4385,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>310</v>
       </c>
@@ -4047,7 +4393,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>311</v>
       </c>
@@ -4055,7 +4401,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>312</v>
       </c>
@@ -4063,7 +4409,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>313</v>
       </c>
@@ -4071,7 +4417,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>314</v>
       </c>
@@ -4079,7 +4425,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>315</v>
       </c>
@@ -4087,7 +4433,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>316</v>
       </c>
@@ -4095,7 +4441,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>317</v>
       </c>
@@ -4103,7 +4449,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>248</v>
       </c>
@@ -4111,7 +4457,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>318</v>
       </c>
@@ -4119,7 +4465,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>319</v>
       </c>
@@ -4127,7 +4473,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>320</v>
       </c>
@@ -4135,7 +4481,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>321</v>
       </c>
@@ -4143,7 +4489,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>322</v>
       </c>
@@ -4151,7 +4497,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>323</v>
       </c>
@@ -4159,7 +4505,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>324</v>
       </c>
@@ -4167,7 +4513,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>325</v>
       </c>
@@ -4175,7 +4521,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>326</v>
       </c>
@@ -4183,7 +4529,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>327</v>
       </c>
@@ -4191,7 +4537,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>328</v>
       </c>
@@ -4199,7 +4545,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>329</v>
       </c>
@@ -4207,7 +4553,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>330</v>
       </c>
@@ -4215,7 +4561,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>243</v>
       </c>
@@ -4223,7 +4569,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>331</v>
       </c>
@@ -4231,7 +4577,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>332</v>
       </c>
@@ -4239,7 +4585,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>333</v>
       </c>
@@ -4247,7 +4593,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>334</v>
       </c>
@@ -4255,7 +4601,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>335</v>
       </c>
@@ -4263,7 +4609,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>336</v>
       </c>
@@ -4271,7 +4617,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>337</v>
       </c>
@@ -4279,7 +4625,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>338</v>
       </c>
@@ -4287,7 +4633,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>339</v>
       </c>
@@ -4295,7 +4641,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>340</v>
       </c>
@@ -4303,7 +4649,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>341</v>
       </c>
@@ -4311,7 +4657,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>342</v>
       </c>
@@ -4319,7 +4665,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>343</v>
       </c>
@@ -4327,7 +4673,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>344</v>
       </c>
@@ -4335,7 +4681,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>345</v>
       </c>
@@ -4343,7 +4689,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>346</v>
       </c>
@@ -4351,7 +4697,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>347</v>
       </c>
@@ -4359,7 +4705,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>348</v>
       </c>
@@ -4367,7 +4713,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>349</v>
       </c>
@@ -4375,7 +4721,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>350</v>
       </c>

</xml_diff>

<commit_message>
add StockLisfGet and UserCorssSectionFuncGet
</commit_message>
<xml_diff>
--- a/resource/tsl_tableinfo.xlsx
+++ b/resource/tsl_tableinfo.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9403DE8-2636-4FE3-93F5-F29E01CD046F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97C2D53-F43E-46A3-97FD-202D04349A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FactorID" sheetId="1" r:id="rId1"/>
     <sheet name="IndexNameID" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="483">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1675,6 +1675,13 @@
   </si>
   <si>
     <t>vol_trade</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预案预披露公布日</t>
+  </si>
+  <si>
+    <t>pre_prelanndate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2036,22 +2043,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.21875" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.25" customWidth="1"/>
+    <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2071,7 +2078,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2085,7 +2092,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2099,7 +2106,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2113,7 +2120,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -2127,7 +2134,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -2141,7 +2148,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -2155,7 +2162,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2169,7 +2176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2183,7 +2190,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2197,7 +2204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -2211,7 +2218,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -2225,7 +2232,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2239,7 +2246,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2253,7 +2260,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2267,7 +2274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2281,7 +2288,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2295,7 +2302,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2309,7 +2316,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2323,7 +2330,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2337,7 +2344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2351,7 +2358,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2365,7 +2372,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2379,7 +2386,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2393,7 +2400,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2407,7 +2414,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2428,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2435,7 +2442,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2449,1102 +2456,1116 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>481</v>
+      </c>
+      <c r="B29">
+        <v>18015</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D29">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>47</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>990001</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D29">
-        <v>0</v>
-      </c>
-      <c r="E29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30">
-        <v>990002</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31">
-        <v>990003</v>
+        <v>990002</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B32">
-        <v>990004</v>
+        <v>990003</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B33">
-        <v>990005</v>
+        <v>990004</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B34">
-        <v>990006</v>
+        <v>990005</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B35">
-        <v>990007</v>
+        <v>990006</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B36">
-        <v>990008</v>
+        <v>990007</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="B37">
-        <v>990009</v>
+        <v>990008</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>129</v>
+        <v>68</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B38">
-        <v>990010</v>
+        <v>990009</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>174</v>
+        <v>127</v>
       </c>
       <c r="B39">
-        <v>990011</v>
+        <v>990010</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>172</v>
+        <v>125</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="B40">
-        <v>990012</v>
+        <v>990011</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41">
+        <v>990012</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>71</v>
       </c>
-      <c r="B41">
+      <c r="B42">
         <v>991001</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42">
-        <v>991002</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B43">
-        <v>991003</v>
+        <v>991002</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44">
+        <v>991003</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>80</v>
       </c>
-      <c r="B44">
+      <c r="B45">
         <v>318000</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D44">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>81</v>
-      </c>
-      <c r="B45">
-        <v>318003</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="D45">
         <v>318</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46">
-        <v>318006</v>
+        <v>318003</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46">
         <v>318</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47">
-        <v>318009</v>
+        <v>318006</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D47">
         <v>318</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48">
-        <v>318004</v>
+        <v>318009</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D48">
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49">
+        <v>318004</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>89</v>
       </c>
-      <c r="B49">
+      <c r="B50">
         <v>302001</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D49">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>90</v>
-      </c>
-      <c r="B50">
-        <v>302002</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="D50">
         <v>302</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51">
-        <v>302003</v>
+        <v>302002</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D51">
         <v>302</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52">
-        <v>302004</v>
+        <v>302003</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D52">
         <v>302</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53">
-        <v>302009</v>
+        <v>302004</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D53">
         <v>302</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54">
-        <v>302013</v>
+        <v>302009</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D54">
         <v>302</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55">
-        <v>302014</v>
+        <v>302013</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D55">
         <v>302</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56">
-        <v>302020</v>
+        <v>302014</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D56">
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B57">
-        <v>302028</v>
+        <v>302020</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D57">
         <v>302</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58">
-        <v>302039</v>
+        <v>302028</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D58">
         <v>302</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59">
+        <v>302039</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D59">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>109</v>
       </c>
-      <c r="B59">
+      <c r="B60">
         <v>992001</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C60" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D59">
-        <v>2</v>
-      </c>
-      <c r="E59" t="s">
-        <v>110</v>
-      </c>
-      <c r="F59" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60">
-        <v>992002</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D60">
         <v>2</v>
       </c>
       <c r="E60" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="F60" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B61">
-        <v>992003</v>
+        <v>992002</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D61">
         <v>2</v>
       </c>
       <c r="E61" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B62">
-        <v>992004</v>
+        <v>992003</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F62" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B63">
-        <v>992005</v>
+        <v>992004</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>122</v>
+        <v>14</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64">
+        <v>992005</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s">
         <v>123</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>47</v>
       </c>
-      <c r="B64">
+      <c r="B65">
         <v>993001</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D64">
-        <v>3</v>
-      </c>
-      <c r="E64" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>48</v>
-      </c>
-      <c r="B65">
-        <v>993002</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="D65">
         <v>3</v>
       </c>
       <c r="E65" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>48</v>
+      </c>
+      <c r="B66">
+        <v>993002</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>49</v>
-      </c>
-      <c r="B66">
-        <v>993003</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
       <c r="E66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B67">
+        <v>993003</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>46</v>
-      </c>
-      <c r="B67">
-        <v>993004</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D67">
         <v>3</v>
       </c>
       <c r="E67" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>46</v>
+      </c>
+      <c r="B68">
+        <v>993004</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>50</v>
-      </c>
-      <c r="B68">
-        <v>993005</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D68">
         <v>3</v>
       </c>
       <c r="E68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69">
+        <v>993005</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>51</v>
-      </c>
-      <c r="B69">
-        <v>993006</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="D69">
         <v>3</v>
       </c>
       <c r="E69" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>51</v>
+      </c>
+      <c r="B70">
+        <v>993006</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70">
-        <v>993007</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D70">
         <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B71">
-        <v>993008</v>
+        <v>993007</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D71">
         <v>3</v>
       </c>
       <c r="E71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>993008</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>126</v>
       </c>
-      <c r="B72">
+      <c r="B73">
         <v>993009</v>
       </c>
-      <c r="C72" s="1" t="s">
+      <c r="C73" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D72">
-        <v>4</v>
-      </c>
-      <c r="E72" t="s">
-        <v>128</v>
-      </c>
-      <c r="F72" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>127</v>
-      </c>
-      <c r="B73">
-        <v>993010</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>125</v>
       </c>
       <c r="D73">
         <v>4</v>
       </c>
       <c r="E73" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F73" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B74">
-        <v>993011</v>
+        <v>993010</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
       <c r="D74">
         <v>4</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F74" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B75">
-        <v>993012</v>
+        <v>993011</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D75">
         <v>4</v>
       </c>
       <c r="E75" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F75" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B76">
-        <v>993013</v>
+        <v>993012</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D76">
         <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="F76" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B77">
-        <v>993014</v>
+        <v>993013</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D77">
         <v>4</v>
       </c>
       <c r="E77" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F77" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B78">
-        <v>993015</v>
+        <v>993014</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D78">
         <v>4</v>
       </c>
       <c r="E78" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F78" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B79">
-        <v>993016</v>
+        <v>993015</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D79">
         <v>4</v>
       </c>
       <c r="E79" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F79" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80">
+        <v>993016</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D80">
+        <v>4</v>
+      </c>
+      <c r="E80" t="s">
+        <v>163</v>
+      </c>
+      <c r="F80" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>454</v>
       </c>
-      <c r="B80">
+      <c r="B81">
         <v>132001</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D80">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>456</v>
-      </c>
-      <c r="B81">
-        <v>132002</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>457</v>
       </c>
       <c r="D81">
         <v>132</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B82">
-        <v>132003</v>
+        <v>132002</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="D82">
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
+        <v>458</v>
+      </c>
+      <c r="B83">
+        <v>132003</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D83">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>454</v>
       </c>
-      <c r="B83">
+      <c r="B84">
         <v>131001</v>
       </c>
-      <c r="C83" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D83">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>460</v>
-      </c>
-      <c r="B84">
-        <v>131002</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>469</v>
       </c>
       <c r="D84">
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
       <c r="B85">
-        <v>131003</v>
+        <v>131002</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D85">
         <v>131</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="B86">
-        <v>131004</v>
+        <v>131003</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="D86">
         <v>131</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B87">
-        <v>131005</v>
+        <v>131004</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D87">
         <v>131</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B88">
-        <v>131006</v>
+        <v>131005</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D88">
         <v>131</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B89">
-        <v>131007</v>
+        <v>131006</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D89">
         <v>131</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>464</v>
+      </c>
+      <c r="B90">
+        <v>131007</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D90">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>454</v>
       </c>
-      <c r="B90">
+      <c r="B91">
         <v>130001</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D90">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>472</v>
-      </c>
-      <c r="B91">
-        <v>130004</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="D91">
         <v>130</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B92">
-        <v>130003</v>
+        <v>130004</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D92">
         <v>130</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B93">
-        <v>130002</v>
+        <v>130003</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D93">
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B94">
-        <v>130009</v>
+        <v>130002</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>478</v>
+        <v>467</v>
       </c>
       <c r="D94">
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B95">
-        <v>130010</v>
+        <v>130009</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D95">
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>476</v>
+      </c>
+      <c r="B96">
+        <v>130010</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D96">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>477</v>
       </c>
-      <c r="B96">
+      <c r="B97">
         <v>130011</v>
       </c>
-      <c r="C96" s="1" t="s">
+      <c r="C97" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="D96">
+      <c r="D97">
         <v>130</v>
       </c>
     </row>
@@ -3563,13 +3584,13 @@
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3577,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3585,7 +3606,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3593,7 +3614,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3601,7 +3622,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -3609,7 +3630,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -3617,7 +3638,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -3625,7 +3646,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -3633,7 +3654,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -3641,7 +3662,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -3649,7 +3670,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -3657,7 +3678,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -3665,7 +3686,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>188</v>
       </c>
@@ -3673,7 +3694,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>189</v>
       </c>
@@ -3681,7 +3702,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>192</v>
       </c>
@@ -3689,7 +3710,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>237</v>
       </c>
@@ -3697,7 +3718,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>238</v>
       </c>
@@ -3705,7 +3726,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>240</v>
       </c>
@@ -3713,7 +3734,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>193</v>
       </c>
@@ -3721,7 +3742,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>241</v>
       </c>
@@ -3729,7 +3750,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>194</v>
       </c>
@@ -3737,7 +3758,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>195</v>
       </c>
@@ -3745,7 +3766,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>196</v>
       </c>
@@ -3753,7 +3774,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>197</v>
       </c>
@@ -3761,7 +3782,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>198</v>
       </c>
@@ -3769,7 +3790,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>199</v>
       </c>
@@ -3777,7 +3798,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>200</v>
       </c>
@@ -3785,7 +3806,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>242</v>
       </c>
@@ -3793,7 +3814,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>201</v>
       </c>
@@ -3801,7 +3822,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -3809,7 +3830,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>244</v>
       </c>
@@ -3817,7 +3838,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>203</v>
       </c>
@@ -3825,7 +3846,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>204</v>
       </c>
@@ -3833,7 +3854,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>205</v>
       </c>
@@ -3841,7 +3862,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>206</v>
       </c>
@@ -3849,7 +3870,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>245</v>
       </c>
@@ -3857,7 +3878,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>246</v>
       </c>
@@ -3865,7 +3886,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>247</v>
       </c>
@@ -3873,7 +3894,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>249</v>
       </c>
@@ -3881,7 +3902,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>207</v>
       </c>
@@ -3889,7 +3910,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>250</v>
       </c>
@@ -3897,7 +3918,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>208</v>
       </c>
@@ -3905,7 +3926,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>251</v>
       </c>
@@ -3913,7 +3934,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>252</v>
       </c>
@@ -3921,7 +3942,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>253</v>
       </c>
@@ -3929,7 +3950,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>254</v>
       </c>
@@ -3937,7 +3958,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>255</v>
       </c>
@@ -3945,7 +3966,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>256</v>
       </c>
@@ -3953,7 +3974,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>257</v>
       </c>
@@ -3961,7 +3982,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>258</v>
       </c>
@@ -3969,7 +3990,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>259</v>
       </c>
@@ -3977,7 +3998,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>260</v>
       </c>
@@ -3985,7 +4006,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>261</v>
       </c>
@@ -3993,7 +4014,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>262</v>
       </c>
@@ -4001,7 +4022,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>263</v>
       </c>
@@ -4009,7 +4030,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>264</v>
       </c>
@@ -4017,7 +4038,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>265</v>
       </c>
@@ -4025,7 +4046,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>266</v>
       </c>
@@ -4033,7 +4054,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>267</v>
       </c>
@@ -4041,7 +4062,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>268</v>
       </c>
@@ -4049,7 +4070,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>239</v>
       </c>
@@ -4057,7 +4078,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>269</v>
       </c>
@@ -4065,7 +4086,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>270</v>
       </c>
@@ -4073,7 +4094,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>271</v>
       </c>
@@ -4081,7 +4102,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>272</v>
       </c>
@@ -4089,7 +4110,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>273</v>
       </c>
@@ -4097,7 +4118,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>274</v>
       </c>
@@ -4105,7 +4126,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
@@ -4113,7 +4134,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>276</v>
       </c>
@@ -4121,7 +4142,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>277</v>
       </c>
@@ -4129,7 +4150,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>278</v>
       </c>
@@ -4137,7 +4158,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>279</v>
       </c>
@@ -4145,7 +4166,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>280</v>
       </c>
@@ -4153,7 +4174,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>281</v>
       </c>
@@ -4161,7 +4182,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>282</v>
       </c>
@@ -4169,7 +4190,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>283</v>
       </c>
@@ -4177,7 +4198,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>284</v>
       </c>
@@ -4185,7 +4206,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>285</v>
       </c>
@@ -4193,7 +4214,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>286</v>
       </c>
@@ -4201,7 +4222,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>287</v>
       </c>
@@ -4209,7 +4230,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>288</v>
       </c>
@@ -4217,7 +4238,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>289</v>
       </c>
@@ -4225,7 +4246,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>290</v>
       </c>
@@ -4233,7 +4254,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>291</v>
       </c>
@@ -4241,7 +4262,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>292</v>
       </c>
@@ -4249,7 +4270,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>293</v>
       </c>
@@ -4257,7 +4278,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>294</v>
       </c>
@@ -4265,7 +4286,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>295</v>
       </c>
@@ -4273,7 +4294,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>296</v>
       </c>
@@ -4281,7 +4302,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>297</v>
       </c>
@@ -4289,7 +4310,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>298</v>
       </c>
@@ -4297,7 +4318,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>299</v>
       </c>
@@ -4305,7 +4326,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>300</v>
       </c>
@@ -4313,7 +4334,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>301</v>
       </c>
@@ -4321,7 +4342,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>302</v>
       </c>
@@ -4329,7 +4350,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>303</v>
       </c>
@@ -4337,7 +4358,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>304</v>
       </c>
@@ -4345,7 +4366,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>305</v>
       </c>
@@ -4353,7 +4374,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>306</v>
       </c>
@@ -4361,7 +4382,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>307</v>
       </c>
@@ -4369,7 +4390,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>308</v>
       </c>
@@ -4377,7 +4398,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>309</v>
       </c>
@@ -4385,7 +4406,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>310</v>
       </c>
@@ -4393,7 +4414,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>311</v>
       </c>
@@ -4401,7 +4422,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>312</v>
       </c>
@@ -4409,7 +4430,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>313</v>
       </c>
@@ -4417,7 +4438,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>314</v>
       </c>
@@ -4425,7 +4446,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>315</v>
       </c>
@@ -4433,7 +4454,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>316</v>
       </c>
@@ -4441,7 +4462,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>317</v>
       </c>
@@ -4449,7 +4470,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>248</v>
       </c>
@@ -4457,7 +4478,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>318</v>
       </c>
@@ -4465,7 +4486,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>319</v>
       </c>
@@ -4473,7 +4494,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>320</v>
       </c>
@@ -4481,7 +4502,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>321</v>
       </c>
@@ -4489,7 +4510,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>322</v>
       </c>
@@ -4497,7 +4518,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>323</v>
       </c>
@@ -4505,7 +4526,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>324</v>
       </c>
@@ -4513,7 +4534,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>325</v>
       </c>
@@ -4521,7 +4542,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>326</v>
       </c>
@@ -4529,7 +4550,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>327</v>
       </c>
@@ -4537,7 +4558,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>328</v>
       </c>
@@ -4545,7 +4566,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>329</v>
       </c>
@@ -4553,7 +4574,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>330</v>
       </c>
@@ -4561,7 +4582,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>243</v>
       </c>
@@ -4569,7 +4590,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>331</v>
       </c>
@@ -4577,7 +4598,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>332</v>
       </c>
@@ -4585,7 +4606,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="4" t="s">
         <v>333</v>
       </c>
@@ -4593,7 +4614,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="4" t="s">
         <v>334</v>
       </c>
@@ -4601,7 +4622,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="4" t="s">
         <v>335</v>
       </c>
@@ -4609,7 +4630,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="4" t="s">
         <v>336</v>
       </c>
@@ -4617,7 +4638,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="4" t="s">
         <v>337</v>
       </c>
@@ -4625,7 +4646,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="4" t="s">
         <v>338</v>
       </c>
@@ -4633,7 +4654,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="4" t="s">
         <v>339</v>
       </c>
@@ -4641,7 +4662,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="4" t="s">
         <v>340</v>
       </c>
@@ -4649,7 +4670,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="4" t="s">
         <v>341</v>
       </c>
@@ -4657,7 +4678,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="4" t="s">
         <v>342</v>
       </c>
@@ -4665,7 +4686,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="4" t="s">
         <v>343</v>
       </c>
@@ -4673,7 +4694,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="4" t="s">
         <v>344</v>
       </c>
@@ -4681,7 +4702,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="4" t="s">
         <v>345</v>
       </c>
@@ -4689,7 +4710,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="4" t="s">
         <v>346</v>
       </c>
@@ -4697,7 +4718,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="4" t="s">
         <v>347</v>
       </c>
@@ -4705,7 +4726,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="4" t="s">
         <v>348</v>
       </c>
@@ -4713,7 +4734,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="4" t="s">
         <v>349</v>
       </c>
@@ -4721,7 +4742,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="4" t="s">
         <v>350</v>
       </c>

</xml_diff>

<commit_message>
add fund ashare and closeprice
</commit_message>
<xml_diff>
--- a/resource/tsl_tableinfo.xlsx
+++ b/resource/tsl_tableinfo.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97C2D53-F43E-46A3-97FD-202D04349A36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B493B541-B215-4548-AE50-67A420E0AFA3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FactorID" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="488">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1683,6 +1683,24 @@
   <si>
     <t>pre_prelanndate</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收盘价</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FundIPOC</t>
+  </si>
+  <si>
+    <t>份额</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>shares</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FundNegotiableShares3</t>
   </si>
 </sst>
 </file>
@@ -2043,22 +2061,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.25" customWidth="1"/>
-    <col min="5" max="5" width="20.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2078,7 +2096,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2092,7 +2110,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2106,7 +2124,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
@@ -2120,7 +2138,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>166</v>
       </c>
@@ -2134,7 +2152,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -2148,7 +2166,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>169</v>
       </c>
@@ -2162,7 +2180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2176,7 +2194,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2190,7 +2208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2204,7 +2222,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -2218,7 +2236,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -2232,7 +2250,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2246,7 +2264,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -2260,7 +2278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2274,7 +2292,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2288,7 +2306,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2302,7 +2320,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2316,7 +2334,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2330,7 +2348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2344,7 +2362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -2358,7 +2376,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2372,7 +2390,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2386,7 +2404,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2400,7 +2418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2414,7 +2432,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -2428,7 +2446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -2442,7 +2460,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -2456,7 +2474,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>481</v>
       </c>
@@ -2470,7 +2488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>47</v>
       </c>
@@ -2487,7 +2505,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>48</v>
       </c>
@@ -2504,7 +2522,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -2521,7 +2539,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -2538,7 +2556,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -2555,7 +2573,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2572,7 +2590,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2589,7 +2607,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -2606,7 +2624,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>126</v>
       </c>
@@ -2623,7 +2641,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>127</v>
       </c>
@@ -2640,7 +2658,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -2657,7 +2675,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -2674,7 +2692,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2691,7 +2709,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -2708,7 +2726,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -2725,847 +2743,881 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>483</v>
+      </c>
+      <c r="B45">
+        <v>991004</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>485</v>
+      </c>
+      <c r="B46">
+        <v>991005</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>80</v>
       </c>
-      <c r="B45">
+      <c r="B47">
         <v>318000</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D45">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>81</v>
-      </c>
-      <c r="B46">
-        <v>318003</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D46">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>82</v>
-      </c>
-      <c r="B47">
-        <v>318006</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="D47">
         <v>318</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B48">
-        <v>318009</v>
+        <v>318003</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D48">
         <v>318</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B49">
-        <v>318004</v>
+        <v>318006</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D49">
         <v>318</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50">
+        <v>318009</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D50">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>84</v>
+      </c>
+      <c r="B51">
+        <v>318004</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>89</v>
       </c>
-      <c r="B50">
+      <c r="B52">
         <v>302001</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D50">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>90</v>
-      </c>
-      <c r="B51">
-        <v>302002</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>91</v>
-      </c>
-      <c r="B52">
-        <v>302003</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="D52">
         <v>302</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B53">
-        <v>302004</v>
+        <v>302002</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D53">
         <v>302</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B54">
-        <v>302009</v>
+        <v>302003</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D54">
         <v>302</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B55">
-        <v>302013</v>
+        <v>302004</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D55">
         <v>302</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B56">
-        <v>302014</v>
+        <v>302009</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D56">
         <v>302</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B57">
-        <v>302020</v>
+        <v>302013</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D57">
         <v>302</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B58">
-        <v>302028</v>
+        <v>302014</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D58">
         <v>302</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B59">
-        <v>302039</v>
+        <v>302020</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D59">
         <v>302</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60">
+        <v>302028</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D60">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61">
+        <v>302039</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D61">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>109</v>
       </c>
-      <c r="B60">
+      <c r="B62">
         <v>992001</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D60">
-        <v>2</v>
-      </c>
-      <c r="E60" t="s">
-        <v>110</v>
-      </c>
-      <c r="F60" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61">
-        <v>992002</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D61">
-        <v>2</v>
-      </c>
-      <c r="E61" t="s">
-        <v>116</v>
-      </c>
-      <c r="F61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62">
-        <v>992003</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="D62">
         <v>2</v>
       </c>
       <c r="E62" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="F62" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B63">
-        <v>992004</v>
+        <v>992002</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="D63">
         <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F63" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B64">
-        <v>992005</v>
+        <v>992003</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D64">
         <v>2</v>
       </c>
       <c r="E64" t="s">
+        <v>119</v>
+      </c>
+      <c r="F64" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>120</v>
+      </c>
+      <c r="B65">
+        <v>992004</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>121</v>
+      </c>
+      <c r="F65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>124</v>
+      </c>
+      <c r="B66">
+        <v>992005</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
         <v>123</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F66" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>47</v>
       </c>
-      <c r="B65">
+      <c r="B67">
         <v>993001</v>
       </c>
-      <c r="C65" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D65">
-        <v>3</v>
-      </c>
-      <c r="E65" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>48</v>
-      </c>
-      <c r="B66">
-        <v>993002</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D66">
-        <v>3</v>
-      </c>
-      <c r="E66" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>49</v>
-      </c>
-      <c r="B67">
-        <v>993003</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="D67">
         <v>3</v>
       </c>
       <c r="E67" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B68">
-        <v>993004</v>
+        <v>993002</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D68">
         <v>3</v>
       </c>
       <c r="E68" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B69">
-        <v>993005</v>
+        <v>993003</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D69">
         <v>3</v>
       </c>
       <c r="E69" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B70">
-        <v>993006</v>
+        <v>993004</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D70">
         <v>3</v>
       </c>
       <c r="E70" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B71">
-        <v>993007</v>
+        <v>993005</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D71">
         <v>3</v>
       </c>
       <c r="E71" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B72">
-        <v>993008</v>
+        <v>993006</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D72">
         <v>3</v>
       </c>
       <c r="E72" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>58</v>
+      </c>
+      <c r="B73">
+        <v>993007</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74">
+        <v>993008</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+    <row r="75" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>126</v>
       </c>
-      <c r="B73">
+      <c r="B75">
         <v>993009</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="D73">
-        <v>4</v>
-      </c>
-      <c r="E73" t="s">
-        <v>128</v>
-      </c>
-      <c r="F73" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>127</v>
-      </c>
-      <c r="B74">
-        <v>993010</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D74">
-        <v>4</v>
-      </c>
-      <c r="E74" t="s">
-        <v>132</v>
-      </c>
-      <c r="F74" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>144</v>
-      </c>
-      <c r="B75">
-        <v>993011</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D75">
         <v>4</v>
       </c>
       <c r="E75" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
       <c r="F75" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>127</v>
       </c>
       <c r="B76">
-        <v>993012</v>
+        <v>993010</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="D76">
         <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="F76" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B77">
-        <v>993013</v>
+        <v>993011</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D77">
         <v>4</v>
       </c>
       <c r="E77" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F77" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B78">
-        <v>993014</v>
+        <v>993012</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D78">
         <v>4</v>
       </c>
       <c r="E78" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F78" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B79">
-        <v>993015</v>
+        <v>993013</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D79">
         <v>4</v>
       </c>
       <c r="E79" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="F79" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="15.75" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B80">
-        <v>993016</v>
+        <v>993014</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="D80">
         <v>4</v>
       </c>
       <c r="E80" t="s">
+        <v>156</v>
+      </c>
+      <c r="F80" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>157</v>
+      </c>
+      <c r="B81">
+        <v>993015</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D81">
+        <v>4</v>
+      </c>
+      <c r="E81" t="s">
+        <v>159</v>
+      </c>
+      <c r="F81" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>161</v>
+      </c>
+      <c r="B82">
+        <v>993016</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D82">
+        <v>4</v>
+      </c>
+      <c r="E82" t="s">
         <v>163</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F82" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
+    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>454</v>
       </c>
-      <c r="B81">
+      <c r="B83">
         <v>132001</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D81">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>456</v>
-      </c>
-      <c r="B82">
-        <v>132002</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="D82">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>458</v>
-      </c>
-      <c r="B83">
-        <v>132003</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="D83">
         <v>132</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>456</v>
+      </c>
+      <c r="B84">
+        <v>132002</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D84">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>458</v>
+      </c>
+      <c r="B85">
+        <v>132003</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D85">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>454</v>
       </c>
-      <c r="B84">
+      <c r="B86">
         <v>131001</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D84">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>460</v>
-      </c>
-      <c r="B85">
-        <v>131002</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="D85">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>471</v>
-      </c>
-      <c r="B86">
-        <v>131003</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>470</v>
       </c>
       <c r="D86">
         <v>131</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B87">
-        <v>131004</v>
+        <v>131002</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="D87">
         <v>131</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="B88">
-        <v>131005</v>
+        <v>131003</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="D88">
         <v>131</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B89">
-        <v>131006</v>
+        <v>131004</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D89">
         <v>131</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B90">
-        <v>131007</v>
+        <v>131005</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D90">
         <v>131</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>463</v>
+      </c>
+      <c r="B91">
+        <v>131006</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D91">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>464</v>
+      </c>
+      <c r="B92">
+        <v>131007</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D92">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>454</v>
       </c>
-      <c r="B91">
+      <c r="B93">
         <v>130001</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C93" s="1" t="s">
         <v>455</v>
-      </c>
-      <c r="D91">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>472</v>
-      </c>
-      <c r="B92">
-        <v>130004</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D92">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>473</v>
-      </c>
-      <c r="B93">
-        <v>130003</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>465</v>
       </c>
       <c r="D93">
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B94">
-        <v>130002</v>
+        <v>130004</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D94">
         <v>130</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B95">
-        <v>130009</v>
+        <v>130003</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="D95">
         <v>130</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="B96">
-        <v>130010</v>
+        <v>130002</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>479</v>
+        <v>467</v>
       </c>
       <c r="D96">
         <v>130</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>475</v>
+      </c>
+      <c r="B97">
+        <v>130009</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D97">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>476</v>
+      </c>
+      <c r="B98">
+        <v>130010</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D98">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>477</v>
       </c>
-      <c r="B97">
+      <c r="B99">
         <v>130011</v>
       </c>
-      <c r="C97" s="1" t="s">
+      <c r="C99" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="D97">
+      <c r="D99">
         <v>130</v>
       </c>
     </row>
@@ -3584,13 +3636,13 @@
       <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3598,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3606,7 +3658,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>135</v>
       </c>
@@ -3614,7 +3666,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>136</v>
       </c>
@@ -3622,7 +3674,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -3630,7 +3682,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -3638,7 +3690,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>176</v>
       </c>
@@ -3646,7 +3698,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -3654,7 +3706,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>180</v>
       </c>
@@ -3662,7 +3714,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>182</v>
       </c>
@@ -3670,7 +3722,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>184</v>
       </c>
@@ -3678,7 +3730,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -3686,7 +3738,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>188</v>
       </c>
@@ -3694,7 +3746,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>189</v>
       </c>
@@ -3702,7 +3754,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>192</v>
       </c>
@@ -3710,7 +3762,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>237</v>
       </c>
@@ -3718,7 +3770,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>238</v>
       </c>
@@ -3726,7 +3778,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>240</v>
       </c>
@@ -3734,7 +3786,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>193</v>
       </c>
@@ -3742,7 +3794,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>241</v>
       </c>
@@ -3750,7 +3802,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>194</v>
       </c>
@@ -3758,7 +3810,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>195</v>
       </c>
@@ -3766,7 +3818,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>196</v>
       </c>
@@ -3774,7 +3826,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>197</v>
       </c>
@@ -3782,7 +3834,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>198</v>
       </c>
@@ -3790,7 +3842,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>199</v>
       </c>
@@ -3798,7 +3850,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>200</v>
       </c>
@@ -3806,7 +3858,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>242</v>
       </c>
@@ -3814,7 +3866,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>201</v>
       </c>
@@ -3822,7 +3874,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>202</v>
       </c>
@@ -3830,7 +3882,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>244</v>
       </c>
@@ -3838,7 +3890,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>203</v>
       </c>
@@ -3846,7 +3898,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>204</v>
       </c>
@@ -3854,7 +3906,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>205</v>
       </c>
@@ -3862,7 +3914,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>206</v>
       </c>
@@ -3870,7 +3922,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>245</v>
       </c>
@@ -3878,7 +3930,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>246</v>
       </c>
@@ -3886,7 +3938,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>247</v>
       </c>
@@ -3894,7 +3946,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>249</v>
       </c>
@@ -3902,7 +3954,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>207</v>
       </c>
@@ -3910,7 +3962,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>250</v>
       </c>
@@ -3918,7 +3970,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>208</v>
       </c>
@@ -3926,7 +3978,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>251</v>
       </c>
@@ -3934,7 +3986,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>252</v>
       </c>
@@ -3942,7 +3994,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>253</v>
       </c>
@@ -3950,7 +4002,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>254</v>
       </c>
@@ -3958,7 +4010,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>255</v>
       </c>
@@ -3966,7 +4018,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>256</v>
       </c>
@@ -3974,7 +4026,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>257</v>
       </c>
@@ -3982,7 +4034,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>258</v>
       </c>
@@ -3990,7 +4042,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>259</v>
       </c>
@@ -3998,7 +4050,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>260</v>
       </c>
@@ -4006,7 +4058,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>261</v>
       </c>
@@ -4014,7 +4066,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>262</v>
       </c>
@@ -4022,7 +4074,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>263</v>
       </c>
@@ -4030,7 +4082,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>264</v>
       </c>
@@ -4038,7 +4090,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>265</v>
       </c>
@@ -4046,7 +4098,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>266</v>
       </c>
@@ -4054,7 +4106,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>267</v>
       </c>
@@ -4062,7 +4114,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>268</v>
       </c>
@@ -4070,7 +4122,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>239</v>
       </c>
@@ -4078,7 +4130,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>269</v>
       </c>
@@ -4086,7 +4138,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>270</v>
       </c>
@@ -4094,7 +4146,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>271</v>
       </c>
@@ -4102,7 +4154,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>272</v>
       </c>
@@ -4110,7 +4162,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>273</v>
       </c>
@@ -4118,7 +4170,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>274</v>
       </c>
@@ -4126,7 +4178,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
@@ -4134,7 +4186,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>276</v>
       </c>
@@ -4142,7 +4194,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>277</v>
       </c>
@@ -4150,7 +4202,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>278</v>
       </c>
@@ -4158,7 +4210,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>279</v>
       </c>
@@ -4166,7 +4218,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>280</v>
       </c>
@@ -4174,7 +4226,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>281</v>
       </c>
@@ -4182,7 +4234,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>282</v>
       </c>
@@ -4190,7 +4242,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>283</v>
       </c>
@@ -4198,7 +4250,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>284</v>
       </c>
@@ -4206,7 +4258,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>285</v>
       </c>
@@ -4214,7 +4266,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>286</v>
       </c>
@@ -4222,7 +4274,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>287</v>
       </c>
@@ -4230,7 +4282,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>288</v>
       </c>
@@ -4238,7 +4290,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>289</v>
       </c>
@@ -4246,7 +4298,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>290</v>
       </c>
@@ -4254,7 +4306,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>291</v>
       </c>
@@ -4262,7 +4314,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>292</v>
       </c>
@@ -4270,7 +4322,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>293</v>
       </c>
@@ -4278,7 +4330,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>294</v>
       </c>
@@ -4286,7 +4338,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>295</v>
       </c>
@@ -4294,7 +4346,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>296</v>
       </c>
@@ -4302,7 +4354,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>297</v>
       </c>
@@ -4310,7 +4362,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>298</v>
       </c>
@@ -4318,7 +4370,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>299</v>
       </c>
@@ -4326,7 +4378,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>300</v>
       </c>
@@ -4334,7 +4386,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>301</v>
       </c>
@@ -4342,7 +4394,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>302</v>
       </c>
@@ -4350,7 +4402,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>303</v>
       </c>
@@ -4358,7 +4410,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>304</v>
       </c>
@@ -4366,7 +4418,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>305</v>
       </c>
@@ -4374,7 +4426,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>306</v>
       </c>
@@ -4382,7 +4434,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>307</v>
       </c>
@@ -4390,7 +4442,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>308</v>
       </c>
@@ -4398,7 +4450,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>309</v>
       </c>
@@ -4406,7 +4458,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>310</v>
       </c>
@@ -4414,7 +4466,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>311</v>
       </c>
@@ -4422,7 +4474,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>312</v>
       </c>
@@ -4430,7 +4482,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>313</v>
       </c>
@@ -4438,7 +4490,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>314</v>
       </c>
@@ -4446,7 +4498,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>315</v>
       </c>
@@ -4454,7 +4506,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>316</v>
       </c>
@@ -4462,7 +4514,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>317</v>
       </c>
@@ -4470,7 +4522,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>248</v>
       </c>
@@ -4478,7 +4530,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>318</v>
       </c>
@@ -4486,7 +4538,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>319</v>
       </c>
@@ -4494,7 +4546,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>320</v>
       </c>
@@ -4502,7 +4554,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>321</v>
       </c>
@@ -4510,7 +4562,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>322</v>
       </c>
@@ -4518,7 +4570,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>323</v>
       </c>
@@ -4526,7 +4578,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>324</v>
       </c>
@@ -4534,7 +4586,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>325</v>
       </c>
@@ -4542,7 +4594,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>326</v>
       </c>
@@ -4550,7 +4602,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>327</v>
       </c>
@@ -4558,7 +4610,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>328</v>
       </c>
@@ -4566,7 +4618,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>329</v>
       </c>
@@ -4574,7 +4626,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>330</v>
       </c>
@@ -4582,7 +4634,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>243</v>
       </c>
@@ -4590,7 +4642,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>331</v>
       </c>
@@ -4598,7 +4650,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>332</v>
       </c>
@@ -4606,7 +4658,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>333</v>
       </c>
@@ -4614,7 +4666,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>334</v>
       </c>
@@ -4622,7 +4674,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>335</v>
       </c>
@@ -4630,7 +4682,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>336</v>
       </c>
@@ -4638,7 +4690,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>337</v>
       </c>
@@ -4646,7 +4698,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>338</v>
       </c>
@@ -4654,7 +4706,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>339</v>
       </c>
@@ -4662,7 +4714,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>340</v>
       </c>
@@ -4670,7 +4722,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>341</v>
       </c>
@@ -4678,7 +4730,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>342</v>
       </c>
@@ -4686,7 +4738,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>343</v>
       </c>
@@ -4694,7 +4746,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>344</v>
       </c>
@@ -4702,7 +4754,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>345</v>
       </c>
@@ -4710,7 +4762,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>346</v>
       </c>
@@ -4718,7 +4770,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>347</v>
       </c>
@@ -4726,7 +4778,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>348</v>
       </c>
@@ -4734,7 +4786,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>349</v>
       </c>
@@ -4742,7 +4794,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>350</v>
       </c>

</xml_diff>